<commit_message>
Fix typos in NIST_SP-800-171_rev1
</commit_message>
<xml_diff>
--- a/controls/data/catalogs/800-171-source.xlsx
+++ b/controls/data/catalogs/800-171-source.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/codedata/code/govready-q-master/controls/data/catalogs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16215EC5-B435-9840-9999-F02488CBBD80}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB1CB1C-3BAA-924E-AA2A-89AB6BF6BC43}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="100" yWindow="2160" windowWidth="33300" windowHeight="16940" xr2:uid="{C1D987CF-D6E1-D24D-92DB-0B9DE2E09808}"/>
   </bookViews>
@@ -143,9 +143,6 @@
     <t>3.1.19</t>
   </si>
   <si>
-    <t>Encrypt CUI on mobile devices and mobile computing platforms.21</t>
-  </si>
-  <si>
     <t>3.1.20</t>
   </si>
   <si>
@@ -305,9 +302,6 @@
     <t>3.5.3</t>
   </si>
   <si>
-    <t>Use multifactor authentication22 for local and network access23 to privileged accounts and for network access to non-privileged accounts.</t>
-  </si>
-  <si>
     <t>3.5.4</t>
   </si>
   <si>
@@ -615,9 +609,6 @@
   </si>
   <si>
     <t>3.13.12</t>
-  </si>
-  <si>
-    <t>Prohibit remote activation 27 of collaborative computing devices and provide indication of devices in use to users present at the device.</t>
   </si>
   <si>
     <t>3.13.13</t>
@@ -1023,6 +1014,15 @@
   </si>
   <si>
     <t>System monitoring can detect unauthorized use of organizational systems. System monitoring includes external and internal monitoring. System monitoring is an integral part of continuous monitoring and incident response programs; it is achieved through a variety of tools and techniques (e.g., intrusion detection systems, intrusion prevention systems, malicious code protection software, scanning tools, audit record monitoring software, network monitoring software). Output from system monitoring serves as input to continuous monitoring and incident response programs.\n\nUnusual or unauthorized activities or conditions related to inbound and outbound communications traffic include, for example, internal traffic that indicates the presence of malicious code in systems or propagating among system components, the unauthorized exporting of information, or signaling to external systems. Evidence of malicious code is used to identify potentially compromised systems or system components. System monitoring requirements, including the need for specific types of system monitoring, may be referenced in other requirements.\n\nNIST Special Publication 800-94 provides guidance on intrusion detection and prevention systems.</t>
+  </si>
+  <si>
+    <t>Encrypt CUI on mobile devices and mobile computing platforms.</t>
+  </si>
+  <si>
+    <t>Use multifactor authentication22 for local and network access to privileged accounts and for network access to non-privileged accounts.</t>
+  </si>
+  <si>
+    <t>Prohibit remote activation of collaborative computing devices and provide indication of devices in use to users present at the device.</t>
   </si>
 </sst>
 </file>
@@ -1397,8 +1397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35A05608-BEB2-394F-91F8-6CEB7A25F9BC}">
   <dimension ref="A1:C110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="C109" sqref="C109"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -1417,7 +1417,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.2">
@@ -1428,7 +1428,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="195" x14ac:dyDescent="0.2">
@@ -1439,7 +1439,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.2">
@@ -1450,7 +1450,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="120" x14ac:dyDescent="0.2">
@@ -1461,7 +1461,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.2">
@@ -1472,7 +1472,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="90" x14ac:dyDescent="0.2">
@@ -1483,7 +1483,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.2">
@@ -1494,7 +1494,7 @@
         <v>15</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.2">
@@ -1505,7 +1505,7 @@
         <v>17</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="75" x14ac:dyDescent="0.2">
@@ -1516,7 +1516,7 @@
         <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="75" x14ac:dyDescent="0.2">
@@ -1527,7 +1527,7 @@
         <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="105" x14ac:dyDescent="0.2">
@@ -1538,7 +1538,7 @@
         <v>23</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -1549,7 +1549,7 @@
         <v>25</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -1560,7 +1560,7 @@
         <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="90" x14ac:dyDescent="0.2">
@@ -1571,7 +1571,7 @@
         <v>29</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.2">
@@ -1582,7 +1582,7 @@
         <v>31</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.2">
@@ -1593,7 +1593,7 @@
         <v>33</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="150" x14ac:dyDescent="0.2">
@@ -1604,7 +1604,7 @@
         <v>35</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.2">
@@ -1612,1011 +1612,1011 @@
         <v>36</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>37</v>
+        <v>327</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="195" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="C20" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="75" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="C21" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="C22" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="75" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="C23" s="2" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="120" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="C24" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="75" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="C25" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="225" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="C26" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="C27" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="C28" s="2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="C29" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="C30" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="C31" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="75" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="C32" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C33" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="C34" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="180" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="C35" s="2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="165" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="C36" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="120" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="C37" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="75" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="C38" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="90" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="C39" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="90" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="C40" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="C41" s="2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="C42" s="2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="75" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="C43" s="2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="75" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="C44" s="2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="C45" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="135" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>91</v>
+        <v>328</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="75" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="165" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="90" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="75" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="135" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="90" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="90" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="27" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="40" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="150" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="90" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="75" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="75" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="195" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="165" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="135" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="120" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="120" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="75" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="90" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="90" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="120" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="90" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>195</v>
+        <v>329</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="75" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="75" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="150" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="90" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="135" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="195" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>